<commit_message>
Added last game 3 objects
Added crash checks, visuals for executing commands and game tutorials.
Checked code with sonar (also game 1)
</commit_message>
<xml_diff>
--- a/docs/Product backlog.xlsx
+++ b/docs/Product backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="221">
   <si>
     <t>GoRoffaGo</t>
   </si>
@@ -679,6 +679,18 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>Step weergave</t>
+  </si>
+  <si>
+    <t>Als speler wil ik dat bij het uitvoeren van een stap van elke truck wordt weergegeven wat het commando is dat wordt uitgevoerd zodat ik kan zien welke richting de trucks gaan bewegen.</t>
+  </si>
+  <si>
+    <t>Maak in het programma gedeelte zichtbaar welke stappen worden uitgevoerd.</t>
+  </si>
+  <si>
+    <t>Controleer of bij het uitvoeren de commando's worden weergegeven.</t>
   </si>
 </sst>
 </file>
@@ -783,7 +795,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1568,11 +1580,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1797,6 +1822,9 @@
     <xf numFmtId="49" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1965,13 +1993,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>129</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2041,16 +2069,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>129</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>91</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2117,16 +2145,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>112</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2143,11 +2171,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1817595984"/>
-        <c:axId val="1817596528"/>
+        <c:axId val="-1417581760"/>
+        <c:axId val="-1417579584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1817595984"/>
+        <c:axId val="-1417581760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2209,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1817596528"/>
+        <c:crossAx val="-1417579584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2189,7 +2217,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1817596528"/>
+        <c:axId val="-1417579584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2232,7 +2260,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1817595984"/>
+        <c:crossAx val="-1417581760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="35"/>
@@ -3451,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV76"/>
+  <dimension ref="A1:IV77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5351,7 +5379,7 @@
       <c r="Q48" s="16"/>
       <c r="R48" s="17"/>
     </row>
-    <row r="49" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:256" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="36"/>
       <c r="B49" s="41" t="s">
         <v>35</v>
@@ -5391,7 +5419,7 @@
       <c r="Q49" s="16"/>
       <c r="R49" s="17"/>
     </row>
-    <row r="50" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="36">
         <f>A46+1</f>
         <v>29</v>
@@ -5436,9 +5464,9 @@
       <c r="Q50" s="16"/>
       <c r="R50" s="17"/>
     </row>
-    <row r="51" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="36">
-        <f t="shared" ref="A51:A60" si="1">A50+1</f>
+        <f t="shared" ref="A51:A61" si="1">A50+1</f>
         <v>30</v>
       </c>
       <c r="B51" s="41" t="s">
@@ -5481,86 +5509,317 @@
       <c r="Q51" s="16"/>
       <c r="R51" s="17"/>
     </row>
-    <row r="52" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="69">
-        <f t="shared" si="1"/>
-        <v>31</v>
-      </c>
+    <row r="52" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="104"/>
       <c r="B52" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C52" s="71">
+      <c r="C52" s="67">
         <v>4</v>
       </c>
-      <c r="D52" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="F52" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="G52" s="72" t="s">
-        <v>51</v>
-      </c>
-      <c r="H52" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="I52" s="71"/>
-      <c r="J52" s="71">
-        <v>2</v>
-      </c>
-      <c r="K52" s="72" t="s">
-        <v>85</v>
-      </c>
-      <c r="L52" s="71">
-        <v>2</v>
-      </c>
-      <c r="M52" s="73" t="s">
-        <v>54</v>
-      </c>
+      <c r="D52" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="66" t="s">
+        <v>217</v>
+      </c>
+      <c r="F52" s="66" t="s">
+        <v>218</v>
+      </c>
+      <c r="G52" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="H52" s="66" t="s">
+        <v>220</v>
+      </c>
+      <c r="I52" s="67"/>
+      <c r="J52" s="67">
+        <v>3</v>
+      </c>
+      <c r="K52" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="L52" s="67"/>
+      <c r="M52" s="68"/>
       <c r="N52" s="15"/>
       <c r="O52" s="16"/>
       <c r="P52" s="16"/>
       <c r="Q52" s="16"/>
       <c r="R52" s="17"/>
-    </row>
-    <row r="53" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S52" s="100"/>
+      <c r="T52" s="100"/>
+      <c r="U52" s="100"/>
+      <c r="V52" s="100"/>
+      <c r="W52" s="100"/>
+      <c r="X52" s="100"/>
+      <c r="Y52" s="100"/>
+      <c r="Z52" s="100"/>
+      <c r="AA52" s="100"/>
+      <c r="AB52" s="100"/>
+      <c r="AC52" s="100"/>
+      <c r="AD52" s="100"/>
+      <c r="AE52" s="100"/>
+      <c r="AF52" s="100"/>
+      <c r="AG52" s="100"/>
+      <c r="AH52" s="100"/>
+      <c r="AI52" s="100"/>
+      <c r="AJ52" s="100"/>
+      <c r="AK52" s="100"/>
+      <c r="AL52" s="100"/>
+      <c r="AM52" s="100"/>
+      <c r="AN52" s="100"/>
+      <c r="AO52" s="100"/>
+      <c r="AP52" s="100"/>
+      <c r="AQ52" s="100"/>
+      <c r="AR52" s="100"/>
+      <c r="AS52" s="100"/>
+      <c r="AT52" s="100"/>
+      <c r="AU52" s="100"/>
+      <c r="AV52" s="100"/>
+      <c r="AW52" s="100"/>
+      <c r="AX52" s="100"/>
+      <c r="AY52" s="100"/>
+      <c r="AZ52" s="100"/>
+      <c r="BA52" s="100"/>
+      <c r="BB52" s="100"/>
+      <c r="BC52" s="100"/>
+      <c r="BD52" s="100"/>
+      <c r="BE52" s="100"/>
+      <c r="BF52" s="100"/>
+      <c r="BG52" s="100"/>
+      <c r="BH52" s="100"/>
+      <c r="BI52" s="100"/>
+      <c r="BJ52" s="100"/>
+      <c r="BK52" s="100"/>
+      <c r="BL52" s="100"/>
+      <c r="BM52" s="100"/>
+      <c r="BN52" s="100"/>
+      <c r="BO52" s="100"/>
+      <c r="BP52" s="100"/>
+      <c r="BQ52" s="100"/>
+      <c r="BR52" s="100"/>
+      <c r="BS52" s="100"/>
+      <c r="BT52" s="100"/>
+      <c r="BU52" s="100"/>
+      <c r="BV52" s="100"/>
+      <c r="BW52" s="100"/>
+      <c r="BX52" s="100"/>
+      <c r="BY52" s="100"/>
+      <c r="BZ52" s="100"/>
+      <c r="CA52" s="100"/>
+      <c r="CB52" s="100"/>
+      <c r="CC52" s="100"/>
+      <c r="CD52" s="100"/>
+      <c r="CE52" s="100"/>
+      <c r="CF52" s="100"/>
+      <c r="CG52" s="100"/>
+      <c r="CH52" s="100"/>
+      <c r="CI52" s="100"/>
+      <c r="CJ52" s="100"/>
+      <c r="CK52" s="100"/>
+      <c r="CL52" s="100"/>
+      <c r="CM52" s="100"/>
+      <c r="CN52" s="100"/>
+      <c r="CO52" s="100"/>
+      <c r="CP52" s="100"/>
+      <c r="CQ52" s="100"/>
+      <c r="CR52" s="100"/>
+      <c r="CS52" s="100"/>
+      <c r="CT52" s="100"/>
+      <c r="CU52" s="100"/>
+      <c r="CV52" s="100"/>
+      <c r="CW52" s="100"/>
+      <c r="CX52" s="100"/>
+      <c r="CY52" s="100"/>
+      <c r="CZ52" s="100"/>
+      <c r="DA52" s="100"/>
+      <c r="DB52" s="100"/>
+      <c r="DC52" s="100"/>
+      <c r="DD52" s="100"/>
+      <c r="DE52" s="100"/>
+      <c r="DF52" s="100"/>
+      <c r="DG52" s="100"/>
+      <c r="DH52" s="100"/>
+      <c r="DI52" s="100"/>
+      <c r="DJ52" s="100"/>
+      <c r="DK52" s="100"/>
+      <c r="DL52" s="100"/>
+      <c r="DM52" s="100"/>
+      <c r="DN52" s="100"/>
+      <c r="DO52" s="100"/>
+      <c r="DP52" s="100"/>
+      <c r="DQ52" s="100"/>
+      <c r="DR52" s="100"/>
+      <c r="DS52" s="100"/>
+      <c r="DT52" s="100"/>
+      <c r="DU52" s="100"/>
+      <c r="DV52" s="100"/>
+      <c r="DW52" s="100"/>
+      <c r="DX52" s="100"/>
+      <c r="DY52" s="100"/>
+      <c r="DZ52" s="100"/>
+      <c r="EA52" s="100"/>
+      <c r="EB52" s="100"/>
+      <c r="EC52" s="100"/>
+      <c r="ED52" s="100"/>
+      <c r="EE52" s="100"/>
+      <c r="EF52" s="100"/>
+      <c r="EG52" s="100"/>
+      <c r="EH52" s="100"/>
+      <c r="EI52" s="100"/>
+      <c r="EJ52" s="100"/>
+      <c r="EK52" s="100"/>
+      <c r="EL52" s="100"/>
+      <c r="EM52" s="100"/>
+      <c r="EN52" s="100"/>
+      <c r="EO52" s="100"/>
+      <c r="EP52" s="100"/>
+      <c r="EQ52" s="100"/>
+      <c r="ER52" s="100"/>
+      <c r="ES52" s="100"/>
+      <c r="ET52" s="100"/>
+      <c r="EU52" s="100"/>
+      <c r="EV52" s="100"/>
+      <c r="EW52" s="100"/>
+      <c r="EX52" s="100"/>
+      <c r="EY52" s="100"/>
+      <c r="EZ52" s="100"/>
+      <c r="FA52" s="100"/>
+      <c r="FB52" s="100"/>
+      <c r="FC52" s="100"/>
+      <c r="FD52" s="100"/>
+      <c r="FE52" s="100"/>
+      <c r="FF52" s="100"/>
+      <c r="FG52" s="100"/>
+      <c r="FH52" s="100"/>
+      <c r="FI52" s="100"/>
+      <c r="FJ52" s="100"/>
+      <c r="FK52" s="100"/>
+      <c r="FL52" s="100"/>
+      <c r="FM52" s="100"/>
+      <c r="FN52" s="100"/>
+      <c r="FO52" s="100"/>
+      <c r="FP52" s="100"/>
+      <c r="FQ52" s="100"/>
+      <c r="FR52" s="100"/>
+      <c r="FS52" s="100"/>
+      <c r="FT52" s="100"/>
+      <c r="FU52" s="100"/>
+      <c r="FV52" s="100"/>
+      <c r="FW52" s="100"/>
+      <c r="FX52" s="100"/>
+      <c r="FY52" s="100"/>
+      <c r="FZ52" s="100"/>
+      <c r="GA52" s="100"/>
+      <c r="GB52" s="100"/>
+      <c r="GC52" s="100"/>
+      <c r="GD52" s="100"/>
+      <c r="GE52" s="100"/>
+      <c r="GF52" s="100"/>
+      <c r="GG52" s="100"/>
+      <c r="GH52" s="100"/>
+      <c r="GI52" s="100"/>
+      <c r="GJ52" s="100"/>
+      <c r="GK52" s="100"/>
+      <c r="GL52" s="100"/>
+      <c r="GM52" s="100"/>
+      <c r="GN52" s="100"/>
+      <c r="GO52" s="100"/>
+      <c r="GP52" s="100"/>
+      <c r="GQ52" s="100"/>
+      <c r="GR52" s="100"/>
+      <c r="GS52" s="100"/>
+      <c r="GT52" s="100"/>
+      <c r="GU52" s="100"/>
+      <c r="GV52" s="100"/>
+      <c r="GW52" s="100"/>
+      <c r="GX52" s="100"/>
+      <c r="GY52" s="100"/>
+      <c r="GZ52" s="100"/>
+      <c r="HA52" s="100"/>
+      <c r="HB52" s="100"/>
+      <c r="HC52" s="100"/>
+      <c r="HD52" s="100"/>
+      <c r="HE52" s="100"/>
+      <c r="HF52" s="100"/>
+      <c r="HG52" s="100"/>
+      <c r="HH52" s="100"/>
+      <c r="HI52" s="100"/>
+      <c r="HJ52" s="100"/>
+      <c r="HK52" s="100"/>
+      <c r="HL52" s="100"/>
+      <c r="HM52" s="100"/>
+      <c r="HN52" s="100"/>
+      <c r="HO52" s="100"/>
+      <c r="HP52" s="100"/>
+      <c r="HQ52" s="100"/>
+      <c r="HR52" s="100"/>
+      <c r="HS52" s="100"/>
+      <c r="HT52" s="100"/>
+      <c r="HU52" s="100"/>
+      <c r="HV52" s="100"/>
+      <c r="HW52" s="100"/>
+      <c r="HX52" s="100"/>
+      <c r="HY52" s="100"/>
+      <c r="HZ52" s="100"/>
+      <c r="IA52" s="100"/>
+      <c r="IB52" s="100"/>
+      <c r="IC52" s="100"/>
+      <c r="ID52" s="100"/>
+      <c r="IE52" s="100"/>
+      <c r="IF52" s="100"/>
+      <c r="IG52" s="100"/>
+      <c r="IH52" s="100"/>
+      <c r="II52" s="100"/>
+      <c r="IJ52" s="100"/>
+      <c r="IK52" s="100"/>
+      <c r="IL52" s="100"/>
+      <c r="IM52" s="100"/>
+      <c r="IN52" s="100"/>
+      <c r="IO52" s="100"/>
+      <c r="IP52" s="100"/>
+      <c r="IQ52" s="100"/>
+      <c r="IR52" s="100"/>
+      <c r="IS52" s="100"/>
+      <c r="IT52" s="100"/>
+      <c r="IU52" s="100"/>
+      <c r="IV52" s="100"/>
+    </row>
+    <row r="53" spans="1:256" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="69">
-        <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="B53" s="74" t="s">
-        <v>25</v>
+        <f>A51+1</f>
+        <v>31</v>
+      </c>
+      <c r="B53" s="70" t="s">
+        <v>40</v>
       </c>
       <c r="C53" s="71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D53" s="72" t="s">
         <v>11</v>
       </c>
       <c r="E53" s="72" t="s">
-        <v>175</v>
+        <v>49</v>
       </c>
       <c r="F53" s="72" t="s">
-        <v>176</v>
+        <v>50</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>177</v>
+        <v>51</v>
       </c>
       <c r="H53" s="72" t="s">
-        <v>178</v>
+        <v>52</v>
       </c>
       <c r="I53" s="71"/>
       <c r="J53" s="71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K53" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L53" s="71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M53" s="73" t="s">
         <v>54</v>
@@ -5571,10 +5830,10 @@
       <c r="Q53" s="16"/>
       <c r="R53" s="17"/>
     </row>
-    <row r="54" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:256" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="69">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B54" s="74" t="s">
         <v>25</v>
@@ -5586,26 +5845,26 @@
         <v>11</v>
       </c>
       <c r="E54" s="72" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F54" s="72" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G54" s="72" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H54" s="72" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I54" s="71"/>
       <c r="J54" s="71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K54" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L54" s="71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M54" s="73" t="s">
         <v>54</v>
@@ -5616,10 +5875,10 @@
       <c r="Q54" s="16"/>
       <c r="R54" s="17"/>
     </row>
-    <row r="55" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="69">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B55" s="74" t="s">
         <v>25</v>
@@ -5631,16 +5890,16 @@
         <v>11</v>
       </c>
       <c r="E55" s="72" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F55" s="72" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G55" s="72" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H55" s="72" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I55" s="71"/>
       <c r="J55" s="71">
@@ -5661,10 +5920,10 @@
       <c r="Q55" s="16"/>
       <c r="R55" s="17"/>
     </row>
-    <row r="56" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="69">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B56" s="74" t="s">
         <v>25</v>
@@ -5676,26 +5935,26 @@
         <v>11</v>
       </c>
       <c r="E56" s="72" t="s">
-        <v>90</v>
+        <v>183</v>
       </c>
       <c r="F56" s="72" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G56" s="72" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H56" s="72" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="I56" s="71"/>
       <c r="J56" s="71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K56" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L56" s="71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M56" s="73" t="s">
         <v>54</v>
@@ -5706,12 +5965,12 @@
       <c r="Q56" s="16"/>
       <c r="R56" s="17"/>
     </row>
-    <row r="57" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="69">
         <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="B57" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="74" t="s">
         <v>25</v>
       </c>
       <c r="C57" s="71">
@@ -5721,29 +5980,29 @@
         <v>11</v>
       </c>
       <c r="E57" s="72" t="s">
-        <v>190</v>
+        <v>90</v>
       </c>
       <c r="F57" s="72" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G57" s="72" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H57" s="72" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I57" s="71"/>
       <c r="J57" s="71">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K57" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L57" s="71">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M57" s="73" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="N57" s="15"/>
       <c r="O57" s="16"/>
@@ -5751,44 +6010,44 @@
       <c r="Q57" s="16"/>
       <c r="R57" s="17"/>
     </row>
-    <row r="58" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:256" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="69">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B58" s="76" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B58" s="75" t="s">
+        <v>25</v>
       </c>
       <c r="C58" s="71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D58" s="72" t="s">
         <v>11</v>
       </c>
       <c r="E58" s="72" t="s">
-        <v>81</v>
+        <v>190</v>
       </c>
       <c r="F58" s="72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G58" s="72" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H58" s="72" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I58" s="71"/>
       <c r="J58" s="71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K58" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L58" s="71">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M58" s="73" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="N58" s="15"/>
       <c r="O58" s="16"/>
@@ -5796,13 +6055,13 @@
       <c r="Q58" s="16"/>
       <c r="R58" s="17"/>
     </row>
-    <row r="59" spans="1:18" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="69">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="B59" s="77" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="B59" s="76" t="s">
+        <v>35</v>
       </c>
       <c r="C59" s="71">
         <v>4</v>
@@ -5811,26 +6070,26 @@
         <v>11</v>
       </c>
       <c r="E59" s="72" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="F59" s="72" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G59" s="72" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H59" s="72" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I59" s="71"/>
       <c r="J59" s="71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K59" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L59" s="71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M59" s="73" t="s">
         <v>54</v>
@@ -5841,13 +6100,13 @@
       <c r="Q59" s="16"/>
       <c r="R59" s="17"/>
     </row>
-    <row r="60" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:256" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="69">
         <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B60" s="78" t="s">
-        <v>35</v>
+        <v>38</v>
+      </c>
+      <c r="B60" s="77" t="s">
+        <v>40</v>
       </c>
       <c r="C60" s="71">
         <v>4</v>
@@ -5856,26 +6115,26 @@
         <v>11</v>
       </c>
       <c r="E60" s="72" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F60" s="72" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G60" s="72" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H60" s="72" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I60" s="71"/>
       <c r="J60" s="71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K60" s="72" t="s">
         <v>85</v>
       </c>
       <c r="L60" s="71">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M60" s="73" t="s">
         <v>54</v>
@@ -5886,100 +6145,125 @@
       <c r="Q60" s="16"/>
       <c r="R60" s="17"/>
     </row>
-    <row r="61" spans="1:18" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:256" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="69">
-        <v>40</v>
-      </c>
-      <c r="B61" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="79">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="B61" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" s="71">
         <v>4</v>
       </c>
-      <c r="D61" s="80" t="s">
+      <c r="D61" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="80" t="s">
-        <v>205</v>
-      </c>
-      <c r="F61" s="80" t="s">
-        <v>206</v>
-      </c>
-      <c r="G61" s="80" t="s">
-        <v>207</v>
-      </c>
-      <c r="H61" s="80" t="s">
-        <v>208</v>
-      </c>
-      <c r="I61" s="79"/>
-      <c r="J61" s="79">
-        <v>5</v>
-      </c>
-      <c r="K61" s="72"/>
-      <c r="L61" s="79"/>
-      <c r="M61" s="81"/>
+      <c r="E61" s="72" t="s">
+        <v>201</v>
+      </c>
+      <c r="F61" s="72" t="s">
+        <v>202</v>
+      </c>
+      <c r="G61" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="H61" s="72" t="s">
+        <v>204</v>
+      </c>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71">
+        <v>1</v>
+      </c>
+      <c r="K61" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="L61" s="71">
+        <v>1</v>
+      </c>
+      <c r="M61" s="73" t="s">
+        <v>54</v>
+      </c>
       <c r="N61" s="15"/>
       <c r="O61" s="16"/>
       <c r="P61" s="16"/>
       <c r="Q61" s="16"/>
       <c r="R61" s="17"/>
     </row>
-    <row r="62" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="82">
-        <f>A60+1</f>
+    <row r="62" spans="1:256" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="69">
         <v>40</v>
       </c>
-      <c r="B62" s="83" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62" s="84">
+      <c r="B62" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="79">
         <v>4</v>
       </c>
-      <c r="D62" s="85" t="s">
-        <v>209</v>
-      </c>
-      <c r="E62" s="85" t="s">
-        <v>209</v>
-      </c>
-      <c r="F62" s="86"/>
-      <c r="G62" s="86"/>
-      <c r="H62" s="86"/>
-      <c r="I62" s="86"/>
-      <c r="J62" s="86">
-        <v>8</v>
-      </c>
-      <c r="K62" s="87"/>
-      <c r="L62" s="86"/>
-      <c r="M62" s="88" t="s">
-        <v>30</v>
-      </c>
+      <c r="D62" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="80" t="s">
+        <v>205</v>
+      </c>
+      <c r="F62" s="80" t="s">
+        <v>206</v>
+      </c>
+      <c r="G62" s="80" t="s">
+        <v>207</v>
+      </c>
+      <c r="H62" s="80" t="s">
+        <v>208</v>
+      </c>
+      <c r="I62" s="79"/>
+      <c r="J62" s="79">
+        <v>5</v>
+      </c>
+      <c r="K62" s="72"/>
+      <c r="L62" s="79"/>
+      <c r="M62" s="81"/>
       <c r="N62" s="15"/>
       <c r="O62" s="16"/>
       <c r="P62" s="16"/>
       <c r="Q62" s="16"/>
       <c r="R62" s="17"/>
     </row>
-    <row r="63" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="89"/>
-      <c r="B63" s="87"/>
-      <c r="C63" s="87"/>
-      <c r="D63" s="87"/>
-      <c r="E63" s="87"/>
-      <c r="F63" s="87"/>
-      <c r="G63" s="87"/>
-      <c r="H63" s="87"/>
-      <c r="I63" s="87"/>
-      <c r="J63" s="87"/>
+    <row r="63" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="82">
+        <f>A61+1</f>
+        <v>40</v>
+      </c>
+      <c r="B63" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" s="84">
+        <v>4</v>
+      </c>
+      <c r="D63" s="85" t="s">
+        <v>209</v>
+      </c>
+      <c r="E63" s="85" t="s">
+        <v>209</v>
+      </c>
+      <c r="F63" s="86"/>
+      <c r="G63" s="86"/>
+      <c r="H63" s="86"/>
+      <c r="I63" s="86"/>
+      <c r="J63" s="86">
+        <v>8</v>
+      </c>
       <c r="K63" s="87"/>
-      <c r="L63" s="87"/>
-      <c r="M63" s="90"/>
+      <c r="L63" s="86"/>
+      <c r="M63" s="88" t="s">
+        <v>30</v>
+      </c>
       <c r="N63" s="15"/>
       <c r="O63" s="16"/>
       <c r="P63" s="16"/>
       <c r="Q63" s="16"/>
       <c r="R63" s="17"/>
     </row>
-    <row r="64" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="89"/>
       <c r="B64" s="87"/>
       <c r="C64" s="87"/>
@@ -6020,59 +6304,59 @@
       <c r="R65" s="17"/>
     </row>
     <row r="66" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="91"/>
-      <c r="B66" s="92"/>
-      <c r="C66" s="92"/>
-      <c r="D66" s="92"/>
-      <c r="E66" s="92"/>
-      <c r="F66" s="92"/>
-      <c r="G66" s="92"/>
-      <c r="H66" s="92"/>
-      <c r="I66" s="92"/>
-      <c r="J66" s="92"/>
-      <c r="K66" s="92"/>
-      <c r="L66" s="92"/>
-      <c r="M66" s="93"/>
+      <c r="A66" s="89"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="87"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="87"/>
+      <c r="F66" s="87"/>
+      <c r="G66" s="87"/>
+      <c r="H66" s="87"/>
+      <c r="I66" s="87"/>
+      <c r="J66" s="87"/>
+      <c r="K66" s="87"/>
+      <c r="L66" s="87"/>
+      <c r="M66" s="90"/>
       <c r="N66" s="15"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16"/>
       <c r="Q66" s="16"/>
       <c r="R66" s="17"/>
     </row>
-    <row r="67" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="94"/>
-      <c r="B67" s="95"/>
-      <c r="C67" s="95"/>
-      <c r="D67" s="95"/>
-      <c r="E67" s="95"/>
-      <c r="F67" s="95"/>
-      <c r="G67" s="95"/>
-      <c r="H67" s="95"/>
-      <c r="I67" s="95"/>
-      <c r="J67" s="95"/>
-      <c r="K67" s="95"/>
-      <c r="L67" s="95"/>
-      <c r="M67" s="95"/>
-      <c r="N67" s="16"/>
+    <row r="67" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="91"/>
+      <c r="B67" s="92"/>
+      <c r="C67" s="92"/>
+      <c r="D67" s="92"/>
+      <c r="E67" s="92"/>
+      <c r="F67" s="92"/>
+      <c r="G67" s="92"/>
+      <c r="H67" s="92"/>
+      <c r="I67" s="92"/>
+      <c r="J67" s="92"/>
+      <c r="K67" s="92"/>
+      <c r="L67" s="92"/>
+      <c r="M67" s="93"/>
+      <c r="N67" s="15"/>
       <c r="O67" s="16"/>
       <c r="P67" s="16"/>
       <c r="Q67" s="16"/>
       <c r="R67" s="17"/>
     </row>
     <row r="68" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="96"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16"/>
-      <c r="K68" s="16"/>
-      <c r="L68" s="16"/>
-      <c r="M68" s="16"/>
+      <c r="A68" s="94"/>
+      <c r="B68" s="95"/>
+      <c r="C68" s="95"/>
+      <c r="D68" s="95"/>
+      <c r="E68" s="95"/>
+      <c r="F68" s="95"/>
+      <c r="G68" s="95"/>
+      <c r="H68" s="95"/>
+      <c r="I68" s="95"/>
+      <c r="J68" s="95"/>
+      <c r="K68" s="95"/>
+      <c r="L68" s="95"/>
+      <c r="M68" s="95"/>
       <c r="N68" s="16"/>
       <c r="O68" s="16"/>
       <c r="P68" s="16"/>
@@ -6220,24 +6504,44 @@
       <c r="R75" s="17"/>
     </row>
     <row r="76" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="97"/>
-      <c r="B76" s="98"/>
-      <c r="C76" s="98"/>
-      <c r="D76" s="98"/>
-      <c r="E76" s="98"/>
-      <c r="F76" s="98"/>
-      <c r="G76" s="98"/>
-      <c r="H76" s="98"/>
-      <c r="I76" s="98"/>
-      <c r="J76" s="98"/>
-      <c r="K76" s="98"/>
-      <c r="L76" s="98"/>
-      <c r="M76" s="98"/>
-      <c r="N76" s="98"/>
-      <c r="O76" s="98"/>
-      <c r="P76" s="98"/>
-      <c r="Q76" s="98"/>
-      <c r="R76" s="99"/>
+      <c r="A76" s="96"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
+      <c r="K76" s="16"/>
+      <c r="L76" s="16"/>
+      <c r="M76" s="16"/>
+      <c r="N76" s="16"/>
+      <c r="O76" s="16"/>
+      <c r="P76" s="16"/>
+      <c r="Q76" s="16"/>
+      <c r="R76" s="17"/>
+    </row>
+    <row r="77" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="97"/>
+      <c r="B77" s="98"/>
+      <c r="C77" s="98"/>
+      <c r="D77" s="98"/>
+      <c r="E77" s="98"/>
+      <c r="F77" s="98"/>
+      <c r="G77" s="98"/>
+      <c r="H77" s="98"/>
+      <c r="I77" s="98"/>
+      <c r="J77" s="98"/>
+      <c r="K77" s="98"/>
+      <c r="L77" s="98"/>
+      <c r="M77" s="98"/>
+      <c r="N77" s="98"/>
+      <c r="O77" s="98"/>
+      <c r="P77" s="98"/>
+      <c r="Q77" s="98"/>
+      <c r="R77" s="99"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6301,27 +6605,27 @@
         <v>2</v>
       </c>
       <c r="B2" s="12">
-        <f>SUM('Product Backlog'!$J1:$J66)</f>
-        <v>129</v>
+        <f>SUM('Product Backlog'!$J1:$J67)</f>
+        <v>132</v>
       </c>
       <c r="C2" s="12">
         <f>B2</f>
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D2" s="12">
         <f>B2-SUM($F2:$F$4)+SUM($G2:$G$4)</f>
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E2" s="12">
-        <f>SUMIF('Product Backlog'!$C1:$C66,$A2,'Product Backlog'!$J1:$J66)</f>
+        <f>SUMIF('Product Backlog'!$C1:$C67,$A2,'Product Backlog'!$J1:$J67)</f>
         <v>38</v>
       </c>
       <c r="F2" s="12">
-        <f>SUMIFS('Product Backlog'!$J1:$J66,'Product Backlog'!$C1:$C66,$A2,'Product Backlog'!$L1:$L66,"&gt;0")</f>
+        <f>SUMIFS('Product Backlog'!$J1:$J67,'Product Backlog'!$C1:$C67,$A2,'Product Backlog'!$L1:$L67,"&gt;0")</f>
         <v>38</v>
       </c>
       <c r="G2" s="12">
-        <f>SUMIF('Product Backlog'!$C1:$C66,$A2,'Product Backlog'!$L1:$L66)</f>
+        <f>SUMIF('Product Backlog'!$C1:$C67,$A2,'Product Backlog'!$L1:$L67)</f>
         <v>35</v>
       </c>
       <c r="H2" s="12"/>
@@ -6339,26 +6643,26 @@
       </c>
       <c r="B3" s="12">
         <f>B2-F2</f>
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C3" s="12">
         <f>C2-E2</f>
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D3" s="12">
         <f>B3-SUM($F3:$F$4)+SUM($G3:$G$4)</f>
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E3" s="12">
-        <f>SUMIF('Product Backlog'!$C1:$C66,$A3,'Product Backlog'!$J1:$J66)</f>
+        <f>SUMIF('Product Backlog'!$C1:$C67,$A3,'Product Backlog'!$J1:$J67)</f>
         <v>50</v>
       </c>
       <c r="F3" s="12">
-        <f>SUMIFS('Product Backlog'!$J1:$J66,'Product Backlog'!$C1:$C66,$A3,'Product Backlog'!$L1:$L66,"&gt;0")</f>
+        <f>SUMIFS('Product Backlog'!$J1:$J67,'Product Backlog'!$C1:$C67,$A3,'Product Backlog'!$L1:$L67,"&gt;0")</f>
         <v>46</v>
       </c>
       <c r="G3" s="12">
-        <f>SUMIF('Product Backlog'!$C1:$C66,$A3,'Product Backlog'!$L1:$L66)</f>
+        <f>SUMIF('Product Backlog'!$C1:$C67,$A3,'Product Backlog'!$L1:$L67)</f>
         <v>36</v>
       </c>
       <c r="H3" s="12"/>
@@ -6376,26 +6680,26 @@
       </c>
       <c r="B4" s="12">
         <f>B3-F3</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C4" s="12">
         <f>C3-E3</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D4" s="12">
         <f>B4-SUM($F4:$F$4)+SUM($G4:$G$4)</f>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E4" s="12">
-        <f>SUMIF('Product Backlog'!$C1:$C66,$A4,'Product Backlog'!$J1:$J66)</f>
-        <v>41</v>
+        <f>SUMIF('Product Backlog'!$C1:$C67,$A4,'Product Backlog'!$J1:$J67)</f>
+        <v>44</v>
       </c>
       <c r="F4" s="12">
-        <f>SUMIFS('Product Backlog'!$J1:$J66,'Product Backlog'!$C1:$C66,$A4,'Product Backlog'!$L1:$L66,"&gt;0")</f>
+        <f>SUMIFS('Product Backlog'!$J1:$J67,'Product Backlog'!$C1:$C67,$A4,'Product Backlog'!$L1:$L67,"&gt;0")</f>
         <v>16</v>
       </c>
       <c r="G4" s="12">
-        <f>SUMIF('Product Backlog'!$C1:$C66,$A4,'Product Backlog'!$L1:$L66)</f>
+        <f>SUMIF('Product Backlog'!$C1:$C67,$A4,'Product Backlog'!$L1:$L67)</f>
         <v>12</v>
       </c>
       <c r="H4" s="12"/>
@@ -6413,7 +6717,7 @@
       </c>
       <c r="B5" s="12">
         <f>B4-F4</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5" s="12">
         <f>C4-E4</f>
@@ -6421,7 +6725,7 @@
       </c>
       <c r="D5" s="12">
         <f>B5</f>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>

</xml_diff>

<commit_message>
Created main menu as game portal
</commit_message>
<xml_diff>
--- a/docs/Product backlog.xlsx
+++ b/docs/Product backlog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="221">
   <si>
     <t>GoRoffaGo</t>
   </si>
@@ -2171,11 +2171,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1417581760"/>
-        <c:axId val="-1417579584"/>
+        <c:axId val="1048243312"/>
+        <c:axId val="1048244944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1417581760"/>
+        <c:axId val="1048243312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2209,7 +2209,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1417579584"/>
+        <c:crossAx val="1048244944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2217,7 +2217,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1417579584"/>
+        <c:axId val="1048244944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,7 +2260,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1417581760"/>
+        <c:crossAx val="1048243312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="35"/>
@@ -3482,7 +3482,7 @@
   <dimension ref="A1:IV77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3761,7 +3761,9 @@
       <c r="J10" s="38">
         <v>1</v>
       </c>
-      <c r="K10" s="38"/>
+      <c r="K10" s="38" t="s">
+        <v>53</v>
+      </c>
       <c r="L10" s="38"/>
       <c r="M10" s="40" t="s">
         <v>30</v>

</xml_diff>